<commit_message>
feat(class)[develop]: backend - fix details in report.
</commit_message>
<xml_diff>
--- a/backend/report.xlsx
+++ b/backend/report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Monday</t>
   </si>
@@ -42,6 +42,60 @@
   </si>
   <si>
     <t>Aug 25th 22</t>
+  </si>
+  <si>
+    <t>Asignaturas</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Inteligencia Artificial</t>
+  </si>
+  <si>
+    <t>SRI</t>
+  </si>
+  <si>
+    <t>Sistema de Recuperacion de Informacion </t>
+  </si>
+  <si>
+    <t>Horario de los turnos</t>
+  </si>
+  <si>
+    <t>1º turno</t>
+  </si>
+  <si>
+    <t>08:00 - 09:30</t>
+  </si>
+  <si>
+    <t>2º turno</t>
+  </si>
+  <si>
+    <t>09:30 - 11:00</t>
+  </si>
+  <si>
+    <t>3º turno</t>
+  </si>
+  <si>
+    <t>11:00 - 12:30</t>
+  </si>
+  <si>
+    <t>4º turno</t>
+  </si>
+  <si>
+    <t>12:30 - 14:00</t>
+  </si>
+  <si>
+    <t>5º turno</t>
+  </si>
+  <si>
+    <t>14:00 - 15:30</t>
+  </si>
+  <si>
+    <t>6º turno</t>
+  </si>
+  <si>
+    <t>15:30 - 17:00</t>
   </si>
   <si>
     <t>Semana 08/08  - 12/08</t>
@@ -66,8 +120,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="4">
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -76,6 +137,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="1"/>
@@ -101,15 +169,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyFont="1" fontId="0"/>
-    <xf applyFont="1" fontId="0" applyAlignment="1">
+    <xf applyFont="1" fontId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyFont="1" fontId="1" applyAlignment="1">
+    <xf applyFont="1" fontId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf applyFont="1" fontId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyFont="1" fontId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -121,18 +192,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="3" spans="4:4">
+    <row r="3" spans="4:10">
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:6">
+      <c r="J3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -148,8 +222,14 @@
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:5">
+      <c r="I4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
@@ -161,6 +241,65 @@
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="10:10">
+      <c r="J9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="9:10">
+      <c r="I10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="9:10">
+      <c r="I11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="9:10">
+      <c r="I12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="9:10">
+      <c r="I13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="9:10">
+      <c r="I14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="9:10">
+      <c r="I15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -170,18 +309,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="3" spans="4:4">
+    <row r="3" spans="4:10">
       <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
+        <v>28</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -197,21 +339,92 @@
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="I4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5">
+        <v>30</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="10:10">
+      <c r="J9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="9:10">
+      <c r="I10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="9:10">
+      <c r="I11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="9:10">
+      <c r="I12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10">
+      <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="9:10">
+      <c r="I14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10">
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:4">

</xml_diff>